<commit_message>
[맘파] RecipeProbabilityTable ID누락 수정
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/RecipeProbabilityTable.xlsx
+++ b/ExcelConverter/ExcelFiles/RecipeProbabilityTable.xlsx
@@ -1419,7 +1419,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="11.14"/>
+    <col customWidth="1" min="2" max="2" width="14.14"/>
     <col customWidth="1" min="3" max="3" width="8.71"/>
     <col customWidth="1" min="4" max="4" width="10.57"/>
     <col customWidth="1" min="5" max="26" width="8.71"/>
@@ -1516,7 +1516,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="5">
-        <v>85.0</v>
+        <v>19.0</v>
       </c>
       <c r="D6" s="3">
         <v>50.0</v>
@@ -1533,7 +1533,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="5">
-        <v>38.0</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="3">
         <v>30.0</v>
@@ -1567,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="5">
-        <v>85.0</v>
+        <v>19.0</v>
       </c>
       <c r="D9" s="3">
         <v>40.0</v>
@@ -1587,7 +1587,7 @@
         <v>16.0</v>
       </c>
       <c r="D10" s="3">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="E10" s="3">
         <v>5.0</v>
@@ -1601,10 +1601,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="5">
-        <v>38.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11" s="3">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="E11" s="3">
         <v>5.0</v>
@@ -1618,10 +1618,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="5">
-        <v>85.0</v>
+        <v>19.0</v>
       </c>
       <c r="D12" s="3">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="E12" s="3">
         <v>5.0</v>
@@ -1635,10 +1635,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="5">
-        <v>39.0</v>
+        <v>5.0</v>
       </c>
       <c r="D13" s="3">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="E13" s="3">
         <v>5.0</v>
@@ -1652,10 +1652,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="5">
-        <v>84.0</v>
+        <v>7.0</v>
       </c>
       <c r="D14" s="3">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="E14" s="3">
         <v>5.0</v>

</xml_diff>